<commit_message>
SNOMED Code to be used for federated encounter report docuemnt. #47
</commit_message>
<xml_diff>
--- a/downloads/GPConnectMessaging-Requirements.xlsx
+++ b/downloads/GPConnectMessaging-Requirements.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="108">
   <si>
     <t xml:space="preserve">Requirement ID</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t xml:space="preserve">GPCM-SD-81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPCM-SD-82</t>
   </si>
 </sst>
 </file>
@@ -456,7 +459,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -470,6 +473,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -555,10 +562,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:C85"/>
+  <dimension ref="B2:C86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C87" activeCellId="0" sqref="C87"/>
+      <selection pane="topLeft" activeCell="C88" activeCellId="0" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1238,6 +1245,14 @@
         <v>106</v>
       </c>
       <c r="C85" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C86" s="5" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>